<commit_message>
BIS-1961: Fix wrong semantic annotation
</commit_message>
<xml_diff>
--- a/server-ro-crate/src/main/resources/reference-from-interoperability-0.2-export.xlsx
+++ b/server-ro-crate/src/main/resources/reference-from-interoperability-0.2-export.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92" count="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90" count="90">
   <si>
     <t>Code</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>https://schema.org/</t>
-  </si>
-  <si>
-    <t>https://schema.org/CreativeWork</t>
   </si>
   <si>
     <t>Mandatory</t>
@@ -132,9 +129,6 @@
   </si>
   <si>
     <t>Organization</t>
-  </si>
-  <si>
-    <t>schema.org</t>
   </si>
   <si>
     <t>https://schema.org/version/28.1</t>
@@ -414,8 +408,8 @@
   </sheetPr>
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0" tabSelected="1">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0" tabSelected="1">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -556,8 +550,10 @@
       <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>https://schema.org/CreativeWork</t>
+        </is>
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
@@ -573,46 +569,46 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>11</v>
@@ -626,29 +622,29 @@
     </row>
     <row r="12" spans="1:22" ht="102">
       <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -664,16 +660,16 @@
         <v>5</v>
       </c>
       <c r="Q12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="4" t="inlineStr">
+        <is>
+          <t>http://datacite.org/schema/kernel-4#title
+https://schema.org/name</t>
+        </is>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="R12" s="4" t="inlineStr">
-        <is>
-          <t>http://datacite.org/schema/kernel-4#title
-https://schema.org/title</t>
-        </is>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15">
@@ -692,17 +688,17 @@
         <v>4</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -717,8 +713,10 @@
       <c r="P13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>37</v>
+      <c r="Q13" s="3" t="inlineStr">
+        <is>
+          <t>schema.org</t>
+        </is>
       </c>
       <c r="R13" s="3" t="inlineStr">
         <is>
@@ -726,7 +724,7 @@
         </is>
       </c>
       <c r="S13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15">
@@ -745,17 +743,17 @@
         <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -790,17 +788,17 @@
         <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -816,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="Q15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
@@ -841,10 +839,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
@@ -853,7 +851,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -869,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R16" s="4" t="inlineStr">
         <is>
@@ -878,7 +876,7 @@
         </is>
       </c>
       <c r="S16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
@@ -897,13 +895,13 @@
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
@@ -923,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
@@ -933,7 +931,7 @@
         </is>
       </c>
       <c r="S17" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
@@ -952,17 +950,17 @@
         <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -978,7 +976,7 @@
         <v>5</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R18" s="3" t="inlineStr">
         <is>
@@ -986,7 +984,7 @@
         </is>
       </c>
       <c r="S18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15">
@@ -1006,7 +1004,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
@@ -1052,17 +1050,17 @@
         <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1078,7 +1076,7 @@
         <v>5</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
@@ -1087,7 +1085,7 @@
         </is>
       </c>
       <c r="S20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="135.75">
@@ -1106,10 +1104,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
@@ -1118,7 +1116,7 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1134,13 +1132,13 @@
         <v>5</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15">
@@ -1159,17 +1157,17 @@
         <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1185,13 +1183,13 @@
         <v>5</v>
       </c>
       <c r="Q22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S22" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="R22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="113.25">
@@ -1210,10 +1208,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
@@ -1222,7 +1220,7 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1238,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R23" s="4" t="inlineStr">
         <is>
@@ -1247,7 +1245,7 @@
         </is>
       </c>
       <c r="S23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15">
@@ -1266,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
@@ -1278,7 +1276,7 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1294,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R24" s="4" t="inlineStr">
         <is>
@@ -1303,7 +1301,7 @@
         </is>
       </c>
       <c r="S24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15"/>
@@ -1343,7 +1341,7 @@
     </row>
     <row r="28" spans="1:22" ht="135.75">
       <c r="A28" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1359,13 +1357,13 @@
         </is>
       </c>
       <c r="G28" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
@@ -1376,46 +1374,46 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="P29" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>11</v>
@@ -1443,17 +1441,17 @@
         <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1469,7 +1467,7 @@
         <v>5</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R30" s="4" t="inlineStr">
         <is>
@@ -1478,7 +1476,7 @@
         </is>
       </c>
       <c r="S30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
@@ -1497,17 +1495,17 @@
         <v>4</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1528,29 +1526,29 @@
     </row>
     <row r="32" spans="1:22" ht="113.25">
       <c r="A32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1566,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R32" s="4" t="inlineStr">
         <is>
@@ -1575,7 +1573,7 @@
         </is>
       </c>
       <c r="S32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15">
@@ -1594,17 +1592,17 @@
         <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1620,7 +1618,7 @@
         <v>5</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R33" s="4" t="inlineStr">
         <is>
@@ -1629,7 +1627,7 @@
         </is>
       </c>
       <c r="S33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15">
@@ -1648,17 +1646,17 @@
         <v>4</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1674,7 +1672,7 @@
         <v>5</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R34" s="4" t="inlineStr">
         <is>
@@ -1683,7 +1681,7 @@
         </is>
       </c>
       <c r="S34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
@@ -1702,13 +1700,13 @@
         <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="inlineStr">
@@ -1749,17 +1747,17 @@
         <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1794,17 +1792,17 @@
         <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -1856,7 +1854,7 @@
     </row>
     <row r="41" spans="1:22" ht="15">
       <c r="A41" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -1875,46 +1873,46 @@
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="P42" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>11</v>
@@ -1928,7 +1926,7 @@
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
@@ -1940,17 +1938,17 @@
         <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -1985,13 +1983,13 @@
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3" t="inlineStr">
@@ -2032,10 +2030,10 @@
         <v>4</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="G45" s="3" t="inlineStr">
         <is>
@@ -2104,7 +2102,7 @@
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -2128,7 +2126,7 @@
         </is>
       </c>
       <c r="I49" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
@@ -2139,46 +2137,46 @@
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="M50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="N50" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O50" s="2" t="s">
+      <c r="P50" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>11</v>
@@ -2206,17 +2204,17 @@
         <v>4</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2232,7 +2230,7 @@
         <v>5</v>
       </c>
       <c r="Q51" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R51" s="4" t="inlineStr">
         <is>
@@ -2241,7 +2239,7 @@
         </is>
       </c>
       <c r="S51" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
@@ -2260,17 +2258,17 @@
         <v>4</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2286,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R52" s="3" t="inlineStr">
         <is>
@@ -2294,7 +2292,7 @@
         </is>
       </c>
       <c r="S52" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15">
@@ -2313,17 +2311,17 @@
         <v>4</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2339,7 +2337,7 @@
         <v>5</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R53" s="3" t="inlineStr">
         <is>
@@ -2347,34 +2345,34 @@
         </is>
       </c>
       <c r="S53" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="15">
       <c r="A54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2411,7 +2409,7 @@
     </row>
     <row r="58" spans="1:22" ht="15">
       <c r="A58" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
@@ -2429,7 +2427,7 @@
     </row>
     <row r="61" spans="1:22" ht="15">
       <c r="A61" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>0</v>
@@ -2438,12 +2436,12 @@
         <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="15">
       <c r="A62" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
@@ -2456,76 +2454,76 @@
         </is>
       </c>
       <c r="D62" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="15"/>
     <row r="64" spans="1:22" ht="13.8">
       <c r="A64" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:22" ht="13.8">
       <c r="A65" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="13.8">
       <c r="A66" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:22" ht="13.8">
       <c r="A67" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="J67" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K67" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M67" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L67" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M67" s="2" t="s">
+      <c r="N67" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O67" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N67" s="2" t="s">
+      <c r="P67" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O67" s="2" t="s">
+      <c r="Q67" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="P67" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q67" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:22" ht="13.8">
@@ -2534,7 +2532,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D68" s="2" t="inlineStr">
         <is>
@@ -2542,13 +2540,13 @@
         </is>
       </c>
       <c r="E68" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G68" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2571,7 +2569,7 @@
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
@@ -2579,13 +2577,13 @@
         </is>
       </c>
       <c r="E69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G69" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -2612,7 +2610,7 @@
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D70" s="2" t="inlineStr">
         <is>
@@ -2620,13 +2618,13 @@
         </is>
       </c>
       <c r="E70" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G70" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2657,58 +2655,58 @@
     </row>
     <row r="72" spans="1:22" ht="13.8">
       <c r="A72" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:22" ht="13.8">
       <c r="A73" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:22" ht="13.8">
       <c r="A74" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:22" ht="13.8">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="J75" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:22" ht="13.8">
@@ -2717,7 +2715,7 @@
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
@@ -2725,13 +2723,13 @@
         </is>
       </c>
       <c r="E76" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G76" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2750,7 +2748,7 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
@@ -2758,13 +2756,13 @@
         </is>
       </c>
       <c r="E77" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G77" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2793,32 +2791,32 @@
     </row>
     <row r="81" spans="1:22" ht="13.8">
       <c r="A81" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:22" ht="13.8">
       <c r="A82" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:22" ht="13.8">
       <c r="A83" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
@@ -2826,7 +2824,7 @@
         </is>
       </c>
       <c r="C83" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
@@ -2834,7 +2832,7 @@
         </is>
       </c>
       <c r="E83" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>6</v>
@@ -2842,7 +2840,7 @@
     </row>
     <row r="84" spans="1:22" ht="13.8">
       <c r="A84" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
@@ -2850,7 +2848,7 @@
         </is>
       </c>
       <c r="C84" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
@@ -2864,7 +2862,7 @@
     </row>
     <row r="85" spans="1:22" ht="13.8">
       <c r="A85" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B85" s="2" t="inlineStr">
         <is>
@@ -2872,7 +2870,7 @@
         </is>
       </c>
       <c r="C85" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D85" s="2" t="inlineStr">
         <is>
@@ -2880,18 +2878,18 @@
         </is>
       </c>
       <c r="E85" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F85" s="2"/>
     </row>
     <row r="87" spans="1:22" ht="13.8">
       <c r="A87" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="13.8">
       <c r="A88" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:22" ht="13.8">
@@ -2901,70 +2899,70 @@
     </row>
     <row r="90" spans="1:22" ht="13.8">
       <c r="A90" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F90" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H90" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="J90" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M90" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N90" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="N90" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q90" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R90" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S90" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R90" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S90" s="2" t="s">
+      <c r="T90" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T90" s="2" t="s">
+      <c r="U90" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V90" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="U90" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V90" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:22" ht="13.8">
@@ -2983,13 +2981,13 @@
         </is>
       </c>
       <c r="E91" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G91" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -3000,7 +2998,7 @@
       </c>
       <c r="K91" s="2"/>
       <c r="L91" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M91" s="2" t="inlineStr">
         <is>
@@ -3016,14 +3014,14 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
       <c r="R91" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="T91" s="2"/>
       <c r="U91" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V91" s="2" t="inlineStr">
         <is>
@@ -3047,13 +3045,13 @@
         </is>
       </c>
       <c r="E92" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G92" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -3064,7 +3062,7 @@
       </c>
       <c r="K92" s="2"/>
       <c r="L92" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M92" s="2" t="inlineStr">
         <is>
@@ -3080,14 +3078,14 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
       <c r="R92" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T92" s="2"/>
       <c r="U92" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V92" s="2" t="inlineStr">
         <is>
@@ -3111,13 +3109,13 @@
         </is>
       </c>
       <c r="E93" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F93" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G93" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -3128,7 +3126,7 @@
       </c>
       <c r="K93" s="2"/>
       <c r="L93" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M93" s="2" t="inlineStr">
         <is>
@@ -3144,14 +3142,14 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
       <c r="R93" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T93" s="2"/>
       <c r="U93" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V93" s="2" t="inlineStr">
         <is>

</xml_diff>